<commit_message>
GestureDetector(       onTap: ( ) { myfun(iii); },
</commit_message>
<xml_diff>
--- a/fluttre .xlsx
+++ b/fluttre .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f3f5af62c6a6f1dd/المستندات/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="476" documentId="8_{609684B2-EED8-49FB-857C-0C148933ACF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{061A5DC7-27C3-4DEB-AEA9-BD899AE02E1A}"/>
+  <xr:revisionPtr revIDLastSave="509" documentId="8_{609684B2-EED8-49FB-857C-0C148933ACF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B592A9B-5F04-4FED-8CAB-DBD80F3FEE8B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{D24CEB46-9FED-4B7E-B9DC-0B0B2305BA4C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="633">
   <si>
     <t>طريقة البد في الفلاتر</t>
   </si>
@@ -2434,12 +2434,140 @@
   <si>
     <t>الدرس 10.11</t>
   </si>
+  <si>
+    <t>دالة  GestureDetector(</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GestureDetector()</t>
+  </si>
+  <si>
+    <t>وتستخدم لكي تجعل الوجدت قابله للضغط بكامل</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> onTap: ( ) { },</t>
+  </si>
+  <si>
+    <t>عنصر الضغط</t>
+  </si>
+  <si>
+    <t>استخدام دالة  GestureDetector(</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GestureDetector(
+      onTap: ( ) {  },
+      child: FractionallySizedBox(</t>
+  </si>
+  <si>
+    <t>تضع الدالة التي تري ان تصح قابل للضغط</t>
+  </si>
+  <si>
+    <t>class _FhadState extends State&lt;Fhad&gt; {
+  change(int ds) {
+    setState(() {
+      nn[ds].hh = !nn[ds].hh;
+    });
+  }
+  @override</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">تضع الفونكشن في هذا المكان علشان لما تسوي
+ لها تحديث اثناء الضغط تقبل 
+وتحط الكود الي هو 
+اليست nn وتفتح [ds]الي تحط فيه رقم العنصر
+وتحط فاريبول علشان نستخدمه في عدد العناصر اليست
+وبعدين يساوي وبعدين علامة  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>علشان اذا ضغط
+مره ثانيه يعكس النتيجه وتحط 
+اليست nn وبعدها  [ds] وتحط نفس الفاريبول
+واخر شي حط الفاريبول في اقواس الفونكشن
+ونحط قيمته في الاستدعاء حق الفونكشن</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> GestureDetector(
+      onTap: ( ) { myfun(iii); },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تروح للصفحه الفرعية وتحط الفونكشن مع القيمه حقت ds
+طبعا القيمه هي فاريبول ثاني </t>
+  </si>
+  <si>
+    <t>final int iii;</t>
+  </si>
+  <si>
+    <t>ولازم تعرف الفاريبول الثاني لى انه رقم صحيح</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Fahad({required this.vartitle,required
+ this.done,required this.myfun,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>required this.iii</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>});</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">وكمان تسويله إعادة التشغيل </t>
+  </si>
+  <si>
+    <t>Fahad(
+                        vartitle: nn[index].titl,
+                        done: nn[index].hh,
+                        myfun: change,
+                        iii:index
+                      );</t>
+  </si>
+  <si>
+    <t>واخيييييرا تروح للصفحه الام وكلاس الي فيه
+ اسدعاء الكلاس وتعرف الفاريبول الي فيه الفونكشن 
+وتحط  index وهو يعني كل عناصر اليست</t>
+  </si>
+  <si>
+    <t>الدرس10.12</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2527,6 +2655,19 @@
       <sz val="11"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2620,7 +2761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2682,14 +2823,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2700,17 +2835,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3031,10 +3175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D101E8F-C8B0-4FAC-ABAE-29C6B4E5ADAC}">
-  <dimension ref="A1:C293"/>
+  <dimension ref="A1:C298"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A283" workbookViewId="0">
-      <selection activeCell="A290" sqref="A290:C290"/>
+    <sheetView rightToLeft="1" topLeftCell="A293" workbookViewId="0">
+      <selection activeCell="A300" sqref="A300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3144,11 +3288,11 @@
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="22" t="s">
         <v>255</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
     </row>
     <row r="18" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -3181,11 +3325,11 @@
       <c r="B22" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
     </row>
     <row r="25" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
@@ -3212,10 +3356,10 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="23"/>
+      <c r="B28" s="29"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
@@ -3274,10 +3418,10 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="23"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -3312,10 +3456,10 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="25"/>
+      <c r="B49" s="23"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
@@ -3334,10 +3478,10 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="25"/>
+      <c r="B52" s="23"/>
       <c r="C52" s="8"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -3387,10 +3531,10 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="24" t="s">
+      <c r="A64" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B64" s="24"/>
+      <c r="B64" s="22"/>
       <c r="C64" s="2" t="s">
         <v>60</v>
       </c>
@@ -3467,11 +3611,11 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="25" t="s">
+      <c r="A73" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
@@ -3529,11 +3673,11 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="24" t="s">
+      <c r="A85" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B85" s="24"/>
-      <c r="C85" s="24"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
@@ -3579,11 +3723,11 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="24" t="s">
+      <c r="A92" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B92" s="24"/>
-      <c r="C92" s="24"/>
+      <c r="B92" s="22"/>
+      <c r="C92" s="22"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
@@ -3610,11 +3754,11 @@
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="24" t="s">
+      <c r="A99" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B99" s="24"/>
-      <c r="C99" s="24"/>
+      <c r="B99" s="22"/>
+      <c r="C99" s="22"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
@@ -3681,10 +3825,10 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="24" t="s">
+      <c r="A108" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="B108" s="24"/>
+      <c r="B108" s="22"/>
       <c r="C108" s="2"/>
     </row>
     <row r="109" spans="1:3" ht="84" x14ac:dyDescent="0.3">
@@ -3726,11 +3870,11 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" s="24" t="s">
+      <c r="A115" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B115" s="24"/>
-      <c r="C115" s="24"/>
+      <c r="B115" s="22"/>
+      <c r="C115" s="22"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
@@ -3765,11 +3909,11 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" s="24" t="s">
+      <c r="A122" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="B122" s="24"/>
-      <c r="C122" s="24"/>
+      <c r="B122" s="22"/>
+      <c r="C122" s="22"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
@@ -3812,11 +3956,11 @@
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="24" t="s">
+      <c r="A129" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="B129" s="24"/>
-      <c r="C129" s="24"/>
+      <c r="B129" s="22"/>
+      <c r="C129" s="22"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
@@ -3843,11 +3987,11 @@
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" s="24" t="s">
+      <c r="A134" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="B134" s="24"/>
-      <c r="C134" s="24"/>
+      <c r="B134" s="22"/>
+      <c r="C134" s="22"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
@@ -3882,11 +4026,11 @@
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" s="24" t="s">
+      <c r="A141" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B141" s="24"/>
-      <c r="C141" s="24"/>
+      <c r="B141" s="22"/>
+      <c r="C141" s="22"/>
     </row>
     <row r="142" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
@@ -3905,11 +4049,11 @@
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="24" t="s">
+      <c r="A146" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="B146" s="24"/>
-      <c r="C146" s="24"/>
+      <c r="B146" s="22"/>
+      <c r="C146" s="22"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
@@ -3945,11 +4089,11 @@
       <c r="A152" s="3"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" s="28" t="s">
+      <c r="A153" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="B153" s="28"/>
-      <c r="C153" s="28"/>
+      <c r="B153" s="26"/>
+      <c r="C153" s="26"/>
     </row>
     <row r="154" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
@@ -3992,11 +4136,11 @@
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160" s="25" t="s">
+      <c r="A160" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="B160" s="25"/>
-      <c r="C160" s="25"/>
+      <c r="B160" s="23"/>
+      <c r="C160" s="23"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
@@ -4031,11 +4175,11 @@
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166" s="25" t="s">
+      <c r="A166" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="B166" s="25"/>
-      <c r="C166" s="25"/>
+      <c r="B166" s="23"/>
+      <c r="C166" s="23"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
@@ -4070,11 +4214,11 @@
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A172" s="25" t="s">
+      <c r="A172" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="B172" s="25"/>
-      <c r="C172" s="25"/>
+      <c r="B172" s="23"/>
+      <c r="C172" s="23"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
@@ -4117,11 +4261,11 @@
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179" s="24" t="s">
+      <c r="A179" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B179" s="24"/>
-      <c r="C179" s="24"/>
+      <c r="B179" s="22"/>
+      <c r="C179" s="22"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
@@ -4145,11 +4289,11 @@
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A186" s="24" t="s">
+      <c r="A186" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="B186" s="24"/>
-      <c r="C186" s="24"/>
+      <c r="B186" s="22"/>
+      <c r="C186" s="22"/>
     </row>
     <row r="187" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
@@ -4203,11 +4347,11 @@
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194" s="28" t="s">
+      <c r="A194" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="B194" s="28"/>
-      <c r="C194" s="28"/>
+      <c r="B194" s="26"/>
+      <c r="C194" s="26"/>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
@@ -4234,11 +4378,11 @@
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200" s="24" t="s">
+      <c r="A200" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="B200" s="24"/>
-      <c r="C200" s="24"/>
+      <c r="B200" s="22"/>
+      <c r="C200" s="22"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
@@ -4273,11 +4417,11 @@
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A206" s="24" t="s">
+      <c r="A206" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="B206" s="24"/>
-      <c r="C206" s="24"/>
+      <c r="B206" s="22"/>
+      <c r="C206" s="22"/>
     </row>
     <row r="207" spans="1:3" ht="70" x14ac:dyDescent="0.3">
       <c r="A207" s="3" t="s">
@@ -4296,11 +4440,11 @@
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A211" s="24" t="s">
+      <c r="A211" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="B211" s="24"/>
-      <c r="C211" s="24"/>
+      <c r="B211" s="22"/>
+      <c r="C211" s="22"/>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
@@ -4346,7 +4490,7 @@
       <c r="A217" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B217" s="26" t="s">
+      <c r="B217" s="24" t="s">
         <v>245</v>
       </c>
     </row>
@@ -4354,7 +4498,7 @@
       <c r="A218" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="B218" s="26"/>
+      <c r="B218" s="24"/>
     </row>
     <row r="219" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="14" t="s">
@@ -4394,11 +4538,11 @@
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A225" s="24" t="s">
+      <c r="A225" s="22" t="s">
         <v>253</v>
       </c>
-      <c r="B225" s="24"/>
-      <c r="C225" s="24"/>
+      <c r="B225" s="22"/>
+      <c r="C225" s="22"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
@@ -4473,11 +4617,11 @@
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A237" s="25" t="s">
+      <c r="A237" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="B237" s="25"/>
-      <c r="C237" s="25"/>
+      <c r="B237" s="23"/>
+      <c r="C237" s="23"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
@@ -4552,11 +4696,11 @@
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A248" s="24" t="s">
+      <c r="A248" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="B248" s="24"/>
-      <c r="C248" s="24"/>
+      <c r="B248" s="22"/>
+      <c r="C248" s="22"/>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
@@ -4575,11 +4719,11 @@
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A253" s="24" t="s">
+      <c r="A253" s="22" t="s">
         <v>314</v>
       </c>
-      <c r="B253" s="24"/>
-      <c r="C253" s="24"/>
+      <c r="B253" s="22"/>
+      <c r="C253" s="22"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
@@ -4606,11 +4750,11 @@
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A258" s="24" t="s">
+      <c r="A258" s="22" t="s">
         <v>461</v>
       </c>
-      <c r="B258" s="24"/>
-      <c r="C258" s="24"/>
+      <c r="B258" s="22"/>
+      <c r="C258" s="22"/>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
@@ -4637,16 +4781,16 @@
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A263" s="24" t="s">
+      <c r="A263" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B263" s="24"/>
+      <c r="B263" s="22"/>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A264" s="25" t="s">
+      <c r="A264" s="23" t="s">
         <v>502</v>
       </c>
-      <c r="B264" s="25"/>
+      <c r="B264" s="23"/>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
@@ -4655,7 +4799,7 @@
       <c r="B265" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="C265" s="26" t="s">
+      <c r="C265" s="24" t="s">
         <v>504</v>
       </c>
     </row>
@@ -4666,7 +4810,7 @@
       <c r="B266" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="C266" s="29"/>
+      <c r="C266" s="25"/>
     </row>
     <row r="267" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A267" s="3" t="s">
@@ -4675,7 +4819,7 @@
       <c r="B267" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="C267" s="29"/>
+      <c r="C267" s="25"/>
     </row>
     <row r="268" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
@@ -4686,11 +4830,11 @@
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A270" s="21" t="s">
+      <c r="A270" s="28" t="s">
         <v>540</v>
       </c>
-      <c r="B270" s="22"/>
-      <c r="C270" s="23"/>
+      <c r="B270" s="30"/>
+      <c r="C270" s="29"/>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" s="19" t="s">
@@ -4740,11 +4884,11 @@
       <c r="A276" s="3"/>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A279" s="24" t="s">
+      <c r="A279" s="22" t="s">
         <v>505</v>
       </c>
-      <c r="B279" s="24"/>
-      <c r="C279" s="24"/>
+      <c r="B279" s="22"/>
+      <c r="C279" s="22"/>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
@@ -4782,11 +4926,11 @@
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A285" s="24" t="s">
+      <c r="A285" s="22" t="s">
         <v>586</v>
       </c>
-      <c r="B285" s="24"/>
-      <c r="C285" s="24"/>
+      <c r="B285" s="22"/>
+      <c r="C285" s="22"/>
     </row>
     <row r="286" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A286" s="3" t="s">
@@ -4795,7 +4939,7 @@
       <c r="B286" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="C286" s="30" t="s">
+      <c r="C286" s="21" t="s">
         <v>589</v>
       </c>
     </row>
@@ -4813,11 +4957,11 @@
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A290" s="24" t="s">
+      <c r="A290" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="B290" s="24"/>
-      <c r="C290" s="24"/>
+      <c r="B290" s="22"/>
+      <c r="C290" s="22"/>
     </row>
     <row r="291" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A291" s="3" t="s">
@@ -4843,27 +4987,48 @@
         <v>599</v>
       </c>
     </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A295" s="22" t="s">
+        <v>614</v>
+      </c>
+      <c r="B295" s="22"/>
+      <c r="C295" s="22"/>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A296" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A297" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A298" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="A285:C285"/>
-    <mergeCell ref="A290:C290"/>
-    <mergeCell ref="A279:C279"/>
-    <mergeCell ref="A258:C258"/>
-    <mergeCell ref="A248:C248"/>
-    <mergeCell ref="A253:C253"/>
-    <mergeCell ref="A264:B264"/>
-    <mergeCell ref="C265:C267"/>
-    <mergeCell ref="A129:C129"/>
-    <mergeCell ref="A134:C134"/>
-    <mergeCell ref="A115:C115"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A211:C211"/>
-    <mergeCell ref="A153:C153"/>
-    <mergeCell ref="A172:C172"/>
-    <mergeCell ref="A146:C146"/>
-    <mergeCell ref="A141:C141"/>
-    <mergeCell ref="A186:C186"/>
-    <mergeCell ref="A194:C194"/>
+  <mergeCells count="43">
+    <mergeCell ref="A295:C295"/>
+    <mergeCell ref="A225:C225"/>
+    <mergeCell ref="A200:C200"/>
+    <mergeCell ref="A237:C237"/>
+    <mergeCell ref="A160:C160"/>
+    <mergeCell ref="A166:C166"/>
+    <mergeCell ref="A179:C179"/>
+    <mergeCell ref="A206:C206"/>
+    <mergeCell ref="B217:B218"/>
     <mergeCell ref="A73:C73"/>
     <mergeCell ref="A122:C122"/>
     <mergeCell ref="A1:B1"/>
@@ -4877,15 +5042,26 @@
     <mergeCell ref="A99:C99"/>
     <mergeCell ref="A92:C92"/>
     <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A129:C129"/>
+    <mergeCell ref="A134:C134"/>
+    <mergeCell ref="A115:C115"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A211:C211"/>
+    <mergeCell ref="A153:C153"/>
+    <mergeCell ref="A172:C172"/>
+    <mergeCell ref="A146:C146"/>
+    <mergeCell ref="A141:C141"/>
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="A194:C194"/>
+    <mergeCell ref="A285:C285"/>
+    <mergeCell ref="A290:C290"/>
+    <mergeCell ref="A279:C279"/>
+    <mergeCell ref="A258:C258"/>
+    <mergeCell ref="A248:C248"/>
+    <mergeCell ref="A253:C253"/>
+    <mergeCell ref="A264:B264"/>
+    <mergeCell ref="C265:C267"/>
     <mergeCell ref="A270:C270"/>
-    <mergeCell ref="A225:C225"/>
-    <mergeCell ref="A200:C200"/>
-    <mergeCell ref="A237:C237"/>
-    <mergeCell ref="A160:C160"/>
-    <mergeCell ref="A166:C166"/>
-    <mergeCell ref="A179:C179"/>
-    <mergeCell ref="A206:C206"/>
-    <mergeCell ref="B217:B218"/>
     <mergeCell ref="A263:B263"/>
   </mergeCells>
   <hyperlinks>
@@ -4901,10 +5077,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A033DF-C58C-4555-B362-B5A41B757F57}">
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:C199"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4923,11 +5099,11 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>290</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="5" spans="1:3" ht="154" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -5002,11 +5178,11 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
@@ -5122,11 +5298,11 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="22" t="s">
         <v>349</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -5169,11 +5345,11 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="22" t="s">
         <v>359</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
     </row>
     <row r="40" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
@@ -5248,11 +5424,11 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="22" t="s">
         <v>379</v>
       </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
     </row>
     <row r="51" spans="1:3" ht="252" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
@@ -5260,11 +5436,11 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="24" t="s">
+      <c r="A53" s="22" t="s">
         <v>328</v>
       </c>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
     </row>
     <row r="54" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
@@ -5363,11 +5539,11 @@
       <c r="B66" s="3"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="24" t="s">
+      <c r="A70" s="22" t="s">
         <v>327</v>
       </c>
-      <c r="B70" s="24"/>
-      <c r="C70" s="24"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
     </row>
     <row r="71" spans="1:3" ht="98" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
@@ -5378,24 +5554,24 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="24" t="s">
+      <c r="A74" s="22" t="s">
         <v>405</v>
       </c>
-      <c r="B74" s="24"/>
-      <c r="C74" s="24"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
     </row>
     <row r="75" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="26" t="s">
+      <c r="A75" s="24" t="s">
         <v>406</v>
       </c>
-      <c r="B75" s="26"/>
+      <c r="B75" s="24"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="24" t="s">
+      <c r="A77" s="22" t="s">
         <v>407</v>
       </c>
-      <c r="B77" s="24"/>
-      <c r="C77" s="24"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="22"/>
     </row>
     <row r="78" spans="1:3" ht="126" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
@@ -5422,11 +5598,11 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="25" t="s">
+      <c r="A82" s="23" t="s">
         <v>417</v>
       </c>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
@@ -5445,11 +5621,11 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="25" t="s">
+      <c r="A87" s="23" t="s">
         <v>422</v>
       </c>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
+      <c r="B87" s="23"/>
+      <c r="C87" s="23"/>
     </row>
     <row r="88" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
@@ -5468,11 +5644,11 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="25" t="s">
+      <c r="A91" s="23" t="s">
         <v>428</v>
       </c>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
     </row>
     <row r="92" spans="1:3" ht="84" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
@@ -5491,11 +5667,11 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="25" t="s">
+      <c r="A96" s="23" t="s">
         <v>432</v>
       </c>
-      <c r="B96" s="25"/>
-      <c r="C96" s="25"/>
+      <c r="B96" s="23"/>
+      <c r="C96" s="23"/>
     </row>
     <row r="97" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
@@ -5538,11 +5714,11 @@
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="24" t="s">
+      <c r="A104" s="22" t="s">
         <v>443</v>
       </c>
-      <c r="B104" s="24"/>
-      <c r="C104" s="24"/>
+      <c r="B104" s="22"/>
+      <c r="C104" s="22"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
@@ -5577,11 +5753,11 @@
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="25" t="s">
+      <c r="A111" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B111" s="25"/>
-      <c r="C111" s="25"/>
+      <c r="B111" s="23"/>
+      <c r="C111" s="23"/>
     </row>
     <row r="112" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
@@ -5600,11 +5776,11 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" s="24" t="s">
+      <c r="A115" s="22" t="s">
         <v>467</v>
       </c>
-      <c r="B115" s="24"/>
-      <c r="C115" s="24"/>
+      <c r="B115" s="22"/>
+      <c r="C115" s="22"/>
     </row>
     <row r="116" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
@@ -5620,11 +5796,11 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="24" t="s">
+      <c r="A119" s="22" t="s">
         <v>471</v>
       </c>
-      <c r="B119" s="24"/>
-      <c r="C119" s="24"/>
+      <c r="B119" s="22"/>
+      <c r="C119" s="22"/>
     </row>
     <row r="120" spans="1:3" ht="70" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
@@ -5657,11 +5833,11 @@
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="25" t="s">
+      <c r="A125" s="23" t="s">
         <v>480</v>
       </c>
-      <c r="B125" s="25"/>
-      <c r="C125" s="25"/>
+      <c r="B125" s="23"/>
+      <c r="C125" s="23"/>
     </row>
     <row r="126" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
@@ -5707,11 +5883,11 @@
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" s="25" t="s">
+      <c r="A132" s="23" t="s">
         <v>492</v>
       </c>
-      <c r="B132" s="25"/>
-      <c r="C132" s="25"/>
+      <c r="B132" s="23"/>
+      <c r="C132" s="23"/>
     </row>
     <row r="133" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
@@ -5746,11 +5922,11 @@
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="22" t="s">
         <v>522</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
@@ -5793,11 +5969,11 @@
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" s="24" t="s">
+      <c r="A149" s="22" t="s">
         <v>533</v>
       </c>
-      <c r="B149" s="24"/>
-      <c r="C149" s="24"/>
+      <c r="B149" s="22"/>
+      <c r="C149" s="22"/>
     </row>
     <row r="150" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
@@ -5824,11 +6000,11 @@
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" s="24" t="s">
+      <c r="A154" s="22" t="s">
         <v>562</v>
       </c>
-      <c r="B154" s="24"/>
-      <c r="C154" s="24"/>
+      <c r="B154" s="22"/>
+      <c r="C154" s="22"/>
     </row>
     <row r="155" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
@@ -5871,11 +6047,11 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" s="24" t="s">
+      <c r="A161" s="22" t="s">
         <v>563</v>
       </c>
-      <c r="B161" s="24"/>
-      <c r="C161" s="24"/>
+      <c r="B161" s="22"/>
+      <c r="C161" s="22"/>
     </row>
     <row r="162" spans="1:3" ht="126" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
@@ -5958,11 +6134,11 @@
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A172" s="25" t="s">
+      <c r="A172" s="23" t="s">
         <v>584</v>
       </c>
-      <c r="B172" s="25"/>
-      <c r="C172" s="25"/>
+      <c r="B172" s="23"/>
+      <c r="C172" s="23"/>
     </row>
     <row r="173" spans="1:3" ht="70" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
@@ -5970,13 +6146,13 @@
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A176" s="24" t="s">
+      <c r="A176" s="22" t="s">
         <v>600</v>
       </c>
-      <c r="B176" s="24"/>
-      <c r="C176" s="24"/>
-    </row>
-    <row r="177" spans="1:2" ht="42" x14ac:dyDescent="0.3">
+      <c r="B176" s="22"/>
+      <c r="C176" s="22"/>
+    </row>
+    <row r="177" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="s">
         <v>601</v>
       </c>
@@ -5984,7 +6160,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="42" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A178" s="3" t="s">
         <v>603</v>
       </c>
@@ -5992,7 +6168,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>605</v>
       </c>
@@ -6000,7 +6176,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="28" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A180" s="3" t="s">
         <v>607</v>
       </c>
@@ -6008,7 +6184,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="42" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A181" s="3" t="s">
         <v>609</v>
       </c>
@@ -6016,7 +6192,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="70" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="70" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>611</v>
       </c>
@@ -6024,23 +6200,121 @@
         <v>612</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B184" s="1" t="s">
         <v>613</v>
       </c>
     </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" s="22" t="s">
+        <v>614</v>
+      </c>
+      <c r="B186" s="22"/>
+      <c r="C186" s="22"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" s="22" t="s">
+        <v>619</v>
+      </c>
+      <c r="B191" s="22"/>
+      <c r="C191" s="22"/>
+    </row>
+    <row r="192" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+      <c r="A192" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="146" x14ac:dyDescent="0.3">
+      <c r="A193" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="B193" s="31" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="42" x14ac:dyDescent="0.3">
+      <c r="A194" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="28" x14ac:dyDescent="0.3">
+      <c r="A196" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="84" x14ac:dyDescent="0.3">
+      <c r="A197" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B199" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="28">
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="A191:C191"/>
+    <mergeCell ref="A132:C132"/>
+    <mergeCell ref="A125:C125"/>
+    <mergeCell ref="A119:C119"/>
+    <mergeCell ref="A115:C115"/>
+    <mergeCell ref="A111:C111"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A50:C50"/>
     <mergeCell ref="A176:C176"/>
     <mergeCell ref="A53:C53"/>
     <mergeCell ref="A70:C70"/>
     <mergeCell ref="A91:C91"/>
     <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A50:C50"/>
     <mergeCell ref="A75:B75"/>
     <mergeCell ref="A77:C77"/>
     <mergeCell ref="A82:C82"/>
@@ -6052,11 +6326,6 @@
     <mergeCell ref="A96:C96"/>
     <mergeCell ref="A104:C104"/>
     <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A132:C132"/>
-    <mergeCell ref="A125:C125"/>
-    <mergeCell ref="A119:C119"/>
-    <mergeCell ref="A115:C115"/>
-    <mergeCell ref="A111:C111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>